<commit_message>
fixed upload farmer metadata
</commit_message>
<xml_diff>
--- a/apps/static/assets/template/Framer_Upload_template.xlsx
+++ b/apps/static/assets/template/Framer_Upload_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WORK\Python_dev\s-tim\apps\static\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C565696F-ACED-45CC-A0A8-02262503EE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917558A-6A2D-44A7-8B8B-9ADDD2764C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1ADBAEC9-2E84-42B3-AEB4-6C807F91EDB2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -61,13 +61,43 @@
   </si>
   <si>
     <t>grpMembership</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>groupementId</t>
+  </si>
+  <si>
+    <t>villageId</t>
+  </si>
+  <si>
+    <t>FSV-0001</t>
+  </si>
+  <si>
+    <t>VAONIRINA</t>
+  </si>
+  <si>
+    <t>ELIA B</t>
+  </si>
+  <si>
+    <t>LAF</t>
+  </si>
+  <si>
+    <t>male/female</t>
+  </si>
+  <si>
+    <t>FALSE/TRUE</t>
+  </si>
+  <si>
+    <t>VSV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,16 +112,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -99,15 +149,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,61 +497,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818C7251-4CB5-4160-9F9C-72E591436C7A}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3</v>
+      </c>
+      <c r="K2" s="5">
+        <v>26299</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated template file for farmer
</commit_message>
<xml_diff>
--- a/apps/static/assets/template/Framer_Upload_template.xlsx
+++ b/apps/static/assets/template/Framer_Upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WORK\Python_dev\s-tim\apps\static\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascal/Projects/github/s-tim/apps/static/assets/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917558A-6A2D-44A7-8B8B-9ADDD2764C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062236D8-7648-6E40-B27E-AF73A058B42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1ADBAEC9-2E84-42B3-AEB4-6C807F91EDB2}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="20740" windowHeight="11320" xr2:uid="{1ADBAEC9-2E84-42B3-AEB4-6C807F91EDB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>firstName</t>
   </si>
@@ -91,6 +91,42 @@
   </si>
   <si>
     <t>VSV</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>PENDING/APPROVED/EXCLUDED</t>
+  </si>
+  <si>
+    <t>statusComment</t>
+  </si>
+  <si>
+    <t>tempManpower</t>
+  </si>
+  <si>
+    <t>permanentManpower</t>
+  </si>
+  <si>
+    <t>hhMembers</t>
+  </si>
+  <si>
+    <t>xsaison_last</t>
+  </si>
+  <si>
+    <t>xsaison_last_but_one</t>
+  </si>
+  <si>
+    <t>xsaison_last_but_two</t>
+  </si>
+  <si>
+    <t>ancienCode</t>
+  </si>
+  <si>
+    <t>registrationStatus</t>
+  </si>
+  <si>
+    <t>ANCIEN/NOUVEAU</t>
   </si>
 </sst>
 </file>
@@ -497,30 +533,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818C7251-4CB5-4160-9F9C-72E591436C7A}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="26.5" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="19" width="16.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="23" width="23.6640625" customWidth="1"/>
+    <col min="24" max="24" width="25.1640625" customWidth="1"/>
+    <col min="25" max="25" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -566,8 +606,38 @@
       <c r="O1" t="s">
         <v>11</v>
       </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -598,6 +668,12 @@
       </c>
       <c r="L2" t="s">
         <v>20</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>